<commit_message>
Acer950 minor change to lockup record
</commit_message>
<xml_diff>
--- a/msff/xls/lockUp{git.xlsx
+++ b/msff/xls/lockUp{git.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA3E5ED-733E-403C-AAED-1AA3B28DB377}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9774586A-D9E3-477C-A999-EA6A1A3D6CF2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16590" yWindow="2085" windowWidth="21240" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3090" yWindow="3435" windowWidth="21240" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lock-up accounting" sheetId="1" r:id="rId1"/>
     <sheet name="shout count" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="139">
   <si>
     <t>CNY. See blog</t>
   </si>
@@ -439,6 +439,9 @@
   </si>
   <si>
     <t>help dad with mlphone slack</t>
+  </si>
+  <si>
+    <t>slept shortly after 12 before a non-school day (CGC counselling)</t>
   </si>
 </sst>
 </file>
@@ -852,7 +855,7 @@
   <dimension ref="A2:G168"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A153" workbookViewId="0">
-      <selection activeCell="G164" sqref="G164"/>
+      <selection activeCell="E164" sqref="E164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3535,11 +3538,19 @@
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B164" s="1"/>
-      <c r="C164" s="8"/>
-      <c r="D164" s="2"/>
-      <c r="E164" s="2"/>
+      <c r="C164" s="8">
+        <v>-1</v>
+      </c>
+      <c r="D164" s="2">
+        <v>45231</v>
+      </c>
+      <c r="E164" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="F164" s="1"/>
-      <c r="G164" s="1"/>
+      <c r="G164" s="1" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B165" s="1"/>
@@ -3570,7 +3581,7 @@
       <c r="D168" s="9"/>
       <c r="E168">
         <f>SUM(B3:B166)+SUM(C3:C166)</f>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F168" s="10" t="s">
         <v>40</v>

</xml_diff>